<commit_message>
fixed bug that cut off last character of task descriptions
</commit_message>
<xml_diff>
--- a/templates/TRG MTA template updated.xlsx
+++ b/templates/TRG MTA template updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\OneDrive\Desktop\Dev Projects\MTA-Converter\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774545BD-1009-4F49-AA3D-428C7B3182D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F1DED7-CD54-41E9-BA5F-8E1318546043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="7755" windowWidth="29040" windowHeight="15840" xr2:uid="{BF392F19-8E36-457E-8500-969E736579D9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="86">
   <si>
     <t>PLSN</t>
   </si>
@@ -252,12 +252,98 @@
 Install turning tool to drain lock.
 Unscrew drain lock using turning tool.</t>
   </si>
+  <si>
+    <t>A350</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>LATCH ASSEMBLY</t>
+  </si>
+  <si>
+    <t>*PINCH WARNING*
+Remove screws from latch assembly
+Remove defective latch assembly                                                                                                                       
+Install new latch assembly
+Secure latch with screws   
+*HAZARDOUS MATERIALS WARNING (PPE)*
+caulk corners</t>
+  </si>
+  <si>
+    <t>Maintainer</t>
+  </si>
+  <si>
+    <t>GMTK, SATS</t>
+  </si>
+  <si>
+    <t>LOCTITE 242
+Rag, Wiping
+Gloves</t>
+  </si>
+  <si>
+    <t>Latch assembly</t>
+  </si>
+  <si>
+    <t>pinch warning</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Screwdriver (GMTK)
+ Drill (SATS)
+Sealant Dispenser (Caulk gun)</t>
+  </si>
+  <si>
+    <t>A660</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>LEFT WING WALL PANEL ASSEMBLY</t>
+  </si>
+  <si>
+    <t>*WEIGHT WARNING* *RIVET WARNING (gloves, eye)*
+Remove rivets from Panel,building,prefabricated,left hinge to endwall
+Remove rivets from Panel,building,prefabricated,left hinge to shelter
+Remove Panel,building,prefabricated,left
+Install new Panel,building,prefabricated,left to shelter. Secure with new rivets
+Secure endwall to Panel,building,prefabricated,left with new rivets</t>
+  </si>
+  <si>
+    <t>BULB SEAL, .748' X .826" X .561", ESS SEAL, ADHESIVE BACK. Hinge seal. Seal tracks, Rivets</t>
+  </si>
+  <si>
+    <t>LOCTITE 242. Sealant 4000 UV
+SEALANT, ADHESIVE (15039)
+Rag, Wiping</t>
+  </si>
+  <si>
+    <t>Panel,building,prefabricated</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Weight Warning (3 Man lift). Drill/ eye warning
+Sealing compound warning</t>
+  </si>
+  <si>
+    <t>Heavy</t>
+  </si>
+  <si>
+    <t>Screwdriver (GMTK)         Drill (SATS)
+Riveter Kit (SATS)
+Drill (SATS)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,8 +378,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +414,12 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -527,7 +625,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -589,6 +687,34 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -612,18 +738,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -956,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CAAB11-A13E-4C91-89E4-59C1E9A7DC85}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -978,46 +1092,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="26" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="21" t="s">
+      <c r="H1" s="37"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21" t="s">
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21" t="s">
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
       <c r="T1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="23"/>
-      <c r="B2" s="25"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1080,13 +1194,13 @@
       <c r="B3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="23" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="23" t="s">
         <v>60</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -1095,7 +1209,7 @@
       <c r="G3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="21" t="s">
         <v>34</v>
       </c>
       <c r="I3" s="10" t="s">
@@ -1142,13 +1256,13 @@
       <c r="B4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="24" t="s">
         <v>31</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="24" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1157,7 +1271,7 @@
       <c r="G4" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="22" t="s">
         <v>42</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1204,13 +1318,13 @@
       <c r="B5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="24" t="s">
         <v>31</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="24" t="s">
         <v>59</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -1219,7 +1333,7 @@
       <c r="G5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -1266,13 +1380,13 @@
       <c r="B6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="24" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="24" t="s">
         <v>61</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1281,7 +1395,7 @@
       <c r="G6" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="22" t="s">
         <v>43</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -1328,13 +1442,13 @@
       <c r="B7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="24" t="s">
         <v>31</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="24" t="s">
         <v>63</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1343,7 +1457,7 @@
       <c r="G7" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="22" t="s">
         <v>56</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1390,13 +1504,13 @@
       <c r="B8" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="24" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="24" t="s">
         <v>62</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -1405,7 +1519,7 @@
       <c r="G8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="22" t="s">
         <v>57</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -1443,6 +1557,130 @@
       </c>
       <c r="T8" s="14" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="27">
+        <v>1</v>
+      </c>
+      <c r="P9" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="Q9" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="R9" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="S9" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="T9" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="M10" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="N10" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="27">
+        <v>3</v>
+      </c>
+      <c r="P10" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="Q10" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="R10" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="S10" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="T10" s="30" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update template and conv col type from int to str where necessary
</commit_message>
<xml_diff>
--- a/templates/TRG MTA template updated.xlsx
+++ b/templates/TRG MTA template updated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\OneDrive\Desktop\Dev Projects\MTA-Converter\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F1DED7-CD54-41E9-BA5F-8E1318546043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B682D5-293A-46E3-984A-D05F24BB6E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="7755" windowWidth="29040" windowHeight="15840" xr2:uid="{BF392F19-8E36-457E-8500-969E736579D9}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>Task Description</t>
   </si>
   <si>
-    <t>Maintainance Class</t>
-  </si>
-  <si>
     <t>Test and Diagnostic Equipment</t>
   </si>
   <si>
@@ -291,11 +288,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Screwdriver (GMTK)
- Drill (SATS)
-Sealant Dispenser (Caulk gun)</t>
-  </si>
-  <si>
     <t>A660</t>
   </si>
   <si>
@@ -337,6 +329,14 @@
     <t>Screwdriver (GMTK)         Drill (SATS)
 Riveter Kit (SATS)
 Drill (SATS)</t>
+  </si>
+  <si>
+    <t>Screwdriver (GMTK)
+Drill (SATS)
+Sealant Dispenser (Caulk gun)</t>
+  </si>
+  <si>
+    <t>Maintenance Class</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1060,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1070,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CAAB11-A13E-4C91-89E4-59C1E9A7DC85}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1079,6 +1079,7 @@
     <col min="3" max="3" width="20.54296875" customWidth="1"/>
     <col min="4" max="4" width="10.26953125" customWidth="1"/>
     <col min="5" max="5" width="43.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" customWidth="1"/>
     <col min="7" max="7" width="10.54296875" customWidth="1"/>
     <col min="8" max="8" width="17.453125" customWidth="1"/>
     <col min="9" max="9" width="11.6328125" customWidth="1"/>
@@ -1142,93 +1143,93 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="T2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="D3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="E3" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="21" t="s">
+      <c r="N3" s="19" t="s">
         <v>34</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="19" t="s">
-        <v>35</v>
       </c>
       <c r="O3" s="20">
         <v>1</v>
@@ -1237,60 +1238,60 @@
         <v>0.2</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="C4" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="D4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="24" t="s">
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="19" t="s">
         <v>32</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" s="19" t="s">
-        <v>33</v>
       </c>
       <c r="O4" s="19">
         <v>1</v>
@@ -1299,60 +1300,60 @@
         <v>0.1</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T4" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>31</v>
-      </c>
       <c r="D5" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="N5" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O5" s="19">
         <v>1</v>
@@ -1361,60 +1362,60 @@
         <v>0.1</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T5" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="C6" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="24" t="s">
-        <v>31</v>
-      </c>
       <c r="D6" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="N6" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O6" s="19">
         <v>2</v>
@@ -1423,60 +1424,60 @@
         <v>0.1</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T6" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="C7" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="24" t="s">
-        <v>31</v>
-      </c>
       <c r="D7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="I7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="L7" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="N7" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O7" s="19">
         <v>2</v>
@@ -1485,60 +1486,60 @@
         <v>0.1</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T7" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="C8" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>31</v>
-      </c>
       <c r="D8" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="L8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="N8" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O8" s="19">
         <v>5</v>
@@ -1547,60 +1548,60 @@
         <v>0.1</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T8" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="C9" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="D9" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="28" t="s">
+      <c r="F9" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="G9" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" s="27" t="s">
+      <c r="J9" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="29" t="s">
+      <c r="L9" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="L9" s="27" t="s">
-        <v>71</v>
-      </c>
       <c r="M9" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N9" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O9" s="27">
         <v>1</v>
@@ -1609,60 +1610,60 @@
         <v>0.1</v>
       </c>
       <c r="Q9" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="R9" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S9" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="T9" s="30" t="s">
         <v>72</v>
-      </c>
-      <c r="R9" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="S9" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="T9" s="30" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="D10" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="F10" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="28" t="s">
+      <c r="K10" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="J10" s="29" t="s">
+      <c r="L10" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="K10" s="29" t="s">
+      <c r="M10" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="L10" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="M10" s="27" t="s">
-        <v>82</v>
-      </c>
       <c r="N10" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O10" s="27">
         <v>3</v>
@@ -1671,21 +1672,21 @@
         <v>0.5</v>
       </c>
       <c r="Q10" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="R10" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="S10" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T10" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="Q14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>